<commit_message>
key change: remove prison guard/corrections officer groups from processed data
</commit_message>
<xml_diff>
--- a/output/staterankings_tocands_all.xlsx
+++ b/output/staterankings_tocands_all.xlsx
@@ -392,243 +392,243 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>AK</t>
         </is>
       </c>
       <c r="B2">
-        <v>15345805.65</v>
+        <v>412111.63</v>
       </c>
       <c r="C2">
-        <v>19618453</v>
+        <v>738516</v>
       </c>
       <c r="D2">
-        <v>782.2128304408101</v>
+        <v>558.0266778241771</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="B3">
-        <v>28269177.8</v>
+        <v>10586763.65</v>
       </c>
       <c r="C3">
-        <v>39148760</v>
+        <v>19618453</v>
       </c>
       <c r="D3">
-        <v>722.0963780206577</v>
+        <v>539.6329491423203</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="B4">
-        <v>488461.63</v>
+        <v>20174621.66</v>
       </c>
       <c r="C4">
-        <v>738516</v>
+        <v>39148760</v>
       </c>
       <c r="D4">
-        <v>661.40967832789</v>
+        <v>515.3323287889579</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
-        <v>47</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RI</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="B5">
-        <v>662496</v>
+        <v>3024580.65</v>
       </c>
       <c r="C5">
-        <v>1056611</v>
+        <v>8881845</v>
       </c>
       <c r="D5">
-        <v>627.000854619155</v>
+        <v>340.5351759685065</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
-        <v>43</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>RI</t>
         </is>
       </c>
       <c r="B6">
-        <v>334059</v>
+        <v>301830</v>
       </c>
       <c r="C6">
-        <v>949495</v>
+        <v>1056611</v>
       </c>
       <c r="D6">
-        <v>351.8280770304215</v>
+        <v>285.6585820136266</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>WA</t>
         </is>
       </c>
       <c r="B7">
-        <v>3038480.65</v>
+        <v>1743449.12</v>
       </c>
       <c r="C7">
-        <v>8881845</v>
+        <v>7294336</v>
       </c>
       <c r="D7">
-        <v>342.100166125394</v>
+        <v>239.0140953199853</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="B8">
-        <v>3761525.48</v>
+        <v>221194</v>
       </c>
       <c r="C8">
-        <v>12791181</v>
+        <v>949495</v>
       </c>
       <c r="D8">
-        <v>294.0717889927443</v>
+        <v>232.9596259064029</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="B9">
-        <v>1859785.56</v>
+        <v>1641724.93</v>
       </c>
       <c r="C9">
-        <v>6830193</v>
+        <v>8413774</v>
       </c>
       <c r="D9">
-        <v>272.2888738283091</v>
+        <v>195.1234879852965</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
       <c r="F9">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>NV</t>
         </is>
       </c>
       <c r="B10">
-        <v>1755299.12</v>
+        <v>568770.29</v>
       </c>
       <c r="C10">
-        <v>7294336</v>
+        <v>2922849</v>
       </c>
       <c r="D10">
-        <v>240.6386434625441</v>
+        <v>194.5944829856076</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
       <c r="F10">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="B11">
-        <v>1641724.93</v>
+        <v>1314897.86</v>
       </c>
       <c r="C11">
-        <v>8413774</v>
+        <v>6830193</v>
       </c>
       <c r="D11">
-        <v>195.1234879852965</v>
+        <v>192.5125483276974</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NV</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="B12">
-        <v>568770.29</v>
+        <v>2177600.08</v>
       </c>
       <c r="C12">
-        <v>2922849</v>
+        <v>12791181</v>
       </c>
       <c r="D12">
-        <v>194.5944829856076</v>
+        <v>170.2423005350327</v>
       </c>
       <c r="E12">
         <v>11</v>
       </c>
       <c r="F12">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -638,13 +638,13 @@
         </is>
       </c>
       <c r="B13">
-        <v>979939.63</v>
+        <v>970959.63</v>
       </c>
       <c r="C13">
         <v>6003435</v>
       </c>
       <c r="D13">
-        <v>163.229822593232</v>
+        <v>161.7340122779709</v>
       </c>
       <c r="E13">
         <v>12</v>
@@ -682,13 +682,13 @@
         </is>
       </c>
       <c r="B15">
-        <v>4145418.02</v>
+        <v>3789218.02</v>
       </c>
       <c r="C15">
         <v>27885195</v>
       </c>
       <c r="D15">
-        <v>148.6601768429448</v>
+        <v>135.8863733963489</v>
       </c>
       <c r="E15">
         <v>14</v>
@@ -748,13 +748,13 @@
         </is>
       </c>
       <c r="B18">
-        <v>1046380</v>
+        <v>935280</v>
       </c>
       <c r="C18">
         <v>9957488</v>
       </c>
       <c r="D18">
-        <v>105.0847362306638</v>
+        <v>93.92730375371779</v>
       </c>
       <c r="E18">
         <v>17</v>
@@ -788,133 +788,133 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>HI</t>
+          <t>OH</t>
         </is>
       </c>
       <c r="B20">
-        <v>110385.94</v>
+        <v>884856.97</v>
       </c>
       <c r="C20">
-        <v>1422029</v>
+        <v>11641879</v>
       </c>
       <c r="D20">
-        <v>77.62566023618365</v>
+        <v>76.0063706210999</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
       <c r="F20">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>OH</t>
+          <t>HI</t>
         </is>
       </c>
       <c r="B21">
-        <v>884856.97</v>
+        <v>105385.94</v>
       </c>
       <c r="C21">
-        <v>11641879</v>
+        <v>1422029</v>
       </c>
       <c r="D21">
-        <v>76.0063706210999</v>
+        <v>74.109557540669</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="B22">
-        <v>263611.19</v>
+        <v>286350</v>
       </c>
       <c r="C22">
-        <v>3581504</v>
+        <v>3918137</v>
       </c>
       <c r="D22">
-        <v>73.60348892532299</v>
+        <v>73.08320255264172</v>
       </c>
       <c r="E22">
         <v>21</v>
       </c>
       <c r="F22">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>NH</t>
         </is>
       </c>
       <c r="B23">
-        <v>286450</v>
+        <v>95120</v>
       </c>
       <c r="C23">
-        <v>3918137</v>
+        <v>1343622</v>
       </c>
       <c r="D23">
-        <v>73.10872488634267</v>
+        <v>70.79372025763199</v>
       </c>
       <c r="E23">
         <v>22</v>
       </c>
       <c r="F23">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>OR</t>
+          <t>CT</t>
         </is>
       </c>
       <c r="B24">
-        <v>297580</v>
+        <v>207291.19</v>
       </c>
       <c r="C24">
-        <v>4081943</v>
+        <v>3581504</v>
       </c>
       <c r="D24">
-        <v>72.90155693011882</v>
+        <v>57.87825170654563</v>
       </c>
       <c r="E24">
         <v>23</v>
       </c>
       <c r="F24">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>NH</t>
+          <t>AL</t>
         </is>
       </c>
       <c r="B25">
-        <v>95120</v>
+        <v>262775.44</v>
       </c>
       <c r="C25">
-        <v>1343622</v>
+        <v>4864680</v>
       </c>
       <c r="D25">
-        <v>70.79372025763199</v>
+        <v>54.01700420171522</v>
       </c>
       <c r="E25">
         <v>24</v>
       </c>
       <c r="F25">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
@@ -924,13 +924,13 @@
         </is>
       </c>
       <c r="B26">
-        <v>420456</v>
+        <v>324995</v>
       </c>
       <c r="C26">
         <v>6090062</v>
       </c>
       <c r="D26">
-        <v>69.03969122153436</v>
+        <v>53.36480975070533</v>
       </c>
       <c r="E26">
         <v>25</v>
@@ -942,111 +942,111 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>WI</t>
         </is>
       </c>
       <c r="B27">
-        <v>262775.44</v>
+        <v>297603</v>
       </c>
       <c r="C27">
-        <v>4864680</v>
+        <v>5778394</v>
       </c>
       <c r="D27">
-        <v>54.01700420171522</v>
+        <v>51.50271857543809</v>
       </c>
       <c r="E27">
         <v>26</v>
       </c>
       <c r="F27">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>WI</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="B28">
-        <v>297603</v>
+        <v>87052.51</v>
       </c>
       <c r="C28">
-        <v>5778394</v>
+        <v>1904760</v>
       </c>
       <c r="D28">
-        <v>51.50271857543809</v>
+        <v>45.70261345261345</v>
       </c>
       <c r="E28">
         <v>27</v>
       </c>
       <c r="F28">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="B29">
-        <v>87052.51</v>
+        <v>302307</v>
       </c>
       <c r="C29">
-        <v>1904760</v>
+        <v>6946685</v>
       </c>
       <c r="D29">
-        <v>45.70261345261345</v>
+        <v>43.51816729850281</v>
       </c>
       <c r="E29">
         <v>28</v>
       </c>
       <c r="F29">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B30">
-        <v>302307</v>
+        <v>43930</v>
       </c>
       <c r="C30">
-        <v>6946685</v>
+        <v>1041732</v>
       </c>
       <c r="D30">
-        <v>43.51816729850281</v>
+        <v>42.17015508787289</v>
       </c>
       <c r="E30">
         <v>29</v>
       </c>
       <c r="F30">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="B31">
-        <v>43930</v>
+        <v>165180</v>
       </c>
       <c r="C31">
-        <v>1041732</v>
+        <v>4081943</v>
       </c>
       <c r="D31">
-        <v>42.17015508787289</v>
+        <v>40.46602316592858</v>
       </c>
       <c r="E31">
         <v>30</v>
       </c>
       <c r="F31">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
@@ -1122,13 +1122,13 @@
         </is>
       </c>
       <c r="B35">
-        <v>91500</v>
+        <v>89500</v>
       </c>
       <c r="C35">
         <v>2908776</v>
       </c>
       <c r="D35">
-        <v>31.45653016939084</v>
+        <v>30.7689557394588</v>
       </c>
       <c r="E35">
         <v>34</v>
@@ -1184,45 +1184,45 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="B38">
-        <v>59252.48</v>
+        <v>146475.19</v>
       </c>
       <c r="C38">
-        <v>3045350</v>
+        <v>10297484</v>
       </c>
       <c r="D38">
-        <v>19.45670612573268</v>
+        <v>14.22436684533814</v>
       </c>
       <c r="E38">
         <v>37</v>
       </c>
       <c r="F38">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>UT</t>
         </is>
       </c>
       <c r="B39">
-        <v>146475.19</v>
+        <v>42152.48</v>
       </c>
       <c r="C39">
-        <v>10297484</v>
+        <v>3045350</v>
       </c>
       <c r="D39">
-        <v>14.22436684533814</v>
+        <v>13.84158799481176</v>
       </c>
       <c r="E39">
         <v>38</v>
       </c>
       <c r="F39">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40">
@@ -1342,13 +1342,13 @@
         </is>
       </c>
       <c r="B45">
-        <v>6800</v>
+        <v>5800</v>
       </c>
       <c r="C45">
         <v>2092434</v>
       </c>
       <c r="D45">
-        <v>3.249803816990165</v>
+        <v>2.7718914909622</v>
       </c>
       <c r="E45">
         <v>44</v>
@@ -1386,13 +1386,13 @@
         </is>
       </c>
       <c r="B47">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="C47">
         <v>624977</v>
       </c>
       <c r="D47">
-        <v>1.360050049841834</v>
+        <v>1.200044161625148</v>
       </c>
       <c r="E47">
         <v>46</v>

</xml_diff>

<commit_message>
comprehensive update - incl. remove ballot initiatives, add yearly charts
</commit_message>
<xml_diff>
--- a/output/staterankings_tocands_all.xlsx
+++ b/output/staterankings_tocands_all.xlsx
@@ -600,7 +600,7 @@
         <v>6830193</v>
       </c>
       <c r="D11">
-        <v>192.5125483276973</v>
+        <v>192.5125483276974</v>
       </c>
       <c r="E11">
         <v>10</v>
@@ -666,7 +666,7 @@
         <v>4663616</v>
       </c>
       <c r="D14">
-        <v>156.9059716751979</v>
+        <v>156.905971675198</v>
       </c>
       <c r="E14">
         <v>13</v>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>87052.50999999999</v>
+        <v>87052.51</v>
       </c>
       <c r="C28">
         <v>1904760</v>

</xml_diff>